<commit_message>
Refactor: extract scenario code.
</commit_message>
<xml_diff>
--- a/input/parameters.xlsx
+++ b/input/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MyProject\Python\2021-05-05-crypto-analyzer\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A6B1C7-2099-4BA9-AD11-A121C735E2AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0EF953-19B6-4560-B0EA-72E4090CA26A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18000" yWindow="3765" windowWidth="17325" windowHeight="19965" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -443,11 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C9B530-6088-40A7-B7AB-B1655394AA59}">
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G78" sqref="G78"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84:B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,6 +3406,9 @@
       <c r="A85">
         <v>84</v>
       </c>
+      <c r="B85" t="s">
+        <v>13</v>
+      </c>
       <c r="C85">
         <v>200000</v>
       </c>
@@ -3441,6 +3444,9 @@
       <c r="A86">
         <v>85</v>
       </c>
+      <c r="B86" t="s">
+        <v>13</v>
+      </c>
       <c r="C86">
         <v>200000</v>
       </c>
@@ -3476,6 +3482,9 @@
       <c r="A87">
         <v>86</v>
       </c>
+      <c r="B87" t="s">
+        <v>13</v>
+      </c>
       <c r="C87">
         <v>200000</v>
       </c>
@@ -3505,6 +3514,38 @@
       </c>
       <c r="L87" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <v>200000</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>14</v>
+      </c>
+      <c r="F88" s="1">
+        <v>43106</v>
+      </c>
+      <c r="G88" s="1">
+        <v>43191</v>
+      </c>
+      <c r="H88">
+        <v>7.7137627095034397E-2</v>
+      </c>
+      <c r="I88">
+        <v>0.147341631456371</v>
+      </c>
+      <c r="J88">
+        <v>3.3881238556444401E-3</v>
+      </c>
+      <c r="K88">
+        <v>0.58523196662204202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature: output pine scripts to draw trading info.
</commit_message>
<xml_diff>
--- a/input/parameters.xlsx
+++ b/input/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MyProject\Python\2021-05-05-crypto-analyzer\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E6B04A-D09B-4A8E-AE10-F405A5BCAE62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299A12AE-090E-4AE4-9FAD-4BD0E4123D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1635" windowWidth="17325" windowHeight="19965" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
+    <workbookView xWindow="9240" yWindow="3375" windowWidth="17325" windowHeight="19965" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="21">
   <si>
     <t>#</t>
   </si>
@@ -449,11 +449,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C9B530-6088-40A7-B7AB-B1655394AA59}">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M84" sqref="M84"/>
+      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3488,9 +3488,6 @@
       <c r="A87">
         <v>86</v>
       </c>
-      <c r="B87" t="s">
-        <v>13</v>
-      </c>
       <c r="C87">
         <v>200000</v>
       </c>
@@ -3561,6 +3558,9 @@
       <c r="A89">
         <v>88</v>
       </c>
+      <c r="B89" t="s">
+        <v>13</v>
+      </c>
       <c r="C89">
         <v>200000</v>
       </c>
@@ -3596,6 +3596,9 @@
       <c r="A90">
         <v>89</v>
       </c>
+      <c r="B90" t="s">
+        <v>13</v>
+      </c>
       <c r="C90">
         <v>200000</v>
       </c>
@@ -3628,6 +3631,9 @@
       <c r="A91">
         <v>90</v>
       </c>
+      <c r="B91" t="s">
+        <v>13</v>
+      </c>
       <c r="C91">
         <v>200000</v>
       </c>
@@ -3663,6 +3669,9 @@
       <c r="A92">
         <v>91</v>
       </c>
+      <c r="B92" t="s">
+        <v>13</v>
+      </c>
       <c r="C92">
         <v>200000</v>
       </c>
@@ -3689,6 +3698,41 @@
       </c>
       <c r="K92">
         <v>2.8670789999999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>13</v>
+      </c>
+      <c r="C93">
+        <v>200000</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="1">
+        <v>44200</v>
+      </c>
+      <c r="G93" s="1">
+        <v>44247</v>
+      </c>
+      <c r="H93">
+        <v>0.61594599999999999</v>
+      </c>
+      <c r="I93">
+        <v>0.99924900000000005</v>
+      </c>
+      <c r="J93">
+        <v>8.1560000000000001E-3</v>
+      </c>
+      <c r="K93">
+        <v>0.74069700000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor: read strategy from input files.
</commit_message>
<xml_diff>
--- a/input/parameters.xlsx
+++ b/input/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MyProject\Python\2021-05-05-crypto-analyzer\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299A12AE-090E-4AE4-9FAD-4BD0E4123D9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA9C5D-FC4A-4D59-B75A-1C8D15AE1668}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="3375" windowWidth="17325" windowHeight="19965" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="34245" windowHeight="19965" xr2:uid="{4E6D9016-1A60-43AB-BF93-1824C6880648}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="25">
   <si>
     <t>#</t>
   </si>
@@ -43,18 +43,6 @@
   </si>
   <si>
     <t>end_date</t>
-  </si>
-  <si>
-    <t>coef_min</t>
-  </si>
-  <si>
-    <t>coef_max</t>
-  </si>
-  <si>
-    <t>coef_a</t>
-  </si>
-  <si>
-    <t>coef_slop</t>
   </si>
   <si>
     <t>ETH</t>
@@ -88,6 +76,30 @@
   </si>
   <si>
     <t>上行情训练数据</t>
+  </si>
+  <si>
+    <t>purchase_stg</t>
+  </si>
+  <si>
+    <t>param_count</t>
+  </si>
+  <si>
+    <t>ExpRatioStrategy</t>
+  </si>
+  <si>
+    <t>LinearRatioStrategy</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
   </si>
 </sst>
 </file>
@@ -131,10 +143,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,11 +463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C9B530-6088-40A7-B7AB-B1655394AA59}">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:N94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G87" sqref="G87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,14 +477,16 @@
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -487,28 +503,34 @@
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>200000</v>
@@ -517,7 +539,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1">
         <v>43952</v>
@@ -525,25 +547,31 @@
       <c r="G2" s="1">
         <v>44317</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4">
+        <v>4</v>
+      </c>
+      <c r="J2">
         <v>0.1</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>1.5</v>
       </c>
-      <c r="J2">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>200000</v>
@@ -552,7 +580,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1">
         <v>43952</v>
@@ -560,25 +588,31 @@
       <c r="G3" s="1">
         <v>44317</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4">
+        <v>4</v>
+      </c>
+      <c r="J3">
         <v>0.2</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1.6</v>
       </c>
-      <c r="J3">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>200000</v>
@@ -587,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F4" s="1">
         <v>43952</v>
@@ -595,25 +629,31 @@
       <c r="G4" s="1">
         <v>44317</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="4">
+        <v>4</v>
+      </c>
+      <c r="J4">
         <v>0.3</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>1.7</v>
       </c>
-      <c r="J4">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>200000</v>
@@ -622,7 +662,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F5" s="1">
         <v>43952</v>
@@ -630,25 +670,31 @@
       <c r="G5" s="1">
         <v>44317</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4">
+        <v>4</v>
+      </c>
+      <c r="J5">
         <v>0.4</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>1.8</v>
       </c>
-      <c r="J5">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>200000</v>
@@ -657,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1">
         <v>43952</v>
@@ -665,25 +711,31 @@
       <c r="G6" s="1">
         <v>44317</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4">
+        <v>4</v>
+      </c>
+      <c r="J6">
         <v>0.5</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>1.9</v>
       </c>
-      <c r="J6">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>200000</v>
@@ -692,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1">
         <v>43952</v>
@@ -700,25 +752,31 @@
       <c r="G7" s="1">
         <v>44317</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7">
         <v>0.6</v>
       </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>7.5000000000000002E-4</v>
-      </c>
       <c r="K7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>200000</v>
@@ -727,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
         <v>43952</v>
@@ -735,25 +793,31 @@
       <c r="G8" s="1">
         <v>44317</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4">
+        <v>4</v>
+      </c>
+      <c r="J8">
         <v>0.7</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>2.1</v>
       </c>
-      <c r="J8">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>200000</v>
@@ -762,7 +826,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F9" s="1">
         <v>43952</v>
@@ -770,25 +834,31 @@
       <c r="G9" s="1">
         <v>44317</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="4">
+        <v>4</v>
+      </c>
+      <c r="J9">
         <v>0.8</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J9">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>200000</v>
@@ -797,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F10" s="1">
         <v>43952</v>
@@ -805,25 +875,31 @@
       <c r="G10" s="1">
         <v>44317</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4">
+        <v>4</v>
+      </c>
+      <c r="J10">
         <v>0.9</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J10">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>200000</v>
@@ -832,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F11" s="1">
         <v>43952</v>
@@ -840,25 +916,31 @@
       <c r="G11" s="1">
         <v>44317</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="4">
+        <v>4</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>2.4</v>
       </c>
-      <c r="J11">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>200000</v>
@@ -867,7 +949,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F12" s="1">
         <v>43952</v>
@@ -875,25 +957,31 @@
       <c r="G12" s="1">
         <v>44317</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="4">
+        <v>4</v>
+      </c>
+      <c r="J12">
         <v>0.1</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>1.5</v>
       </c>
-      <c r="J12">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K12">
+      <c r="L12">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>200000</v>
@@ -902,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F13" s="1">
         <v>43952</v>
@@ -910,25 +998,31 @@
       <c r="G13" s="1">
         <v>44317</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4</v>
+      </c>
+      <c r="J13">
         <v>0.2</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>1.6</v>
       </c>
-      <c r="J13">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K13">
+      <c r="L13">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>200000</v>
@@ -937,7 +1031,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F14" s="1">
         <v>43952</v>
@@ -945,25 +1039,31 @@
       <c r="G14" s="1">
         <v>44317</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="4">
+        <v>4</v>
+      </c>
+      <c r="J14">
         <v>0.3</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>1.7</v>
       </c>
-      <c r="J14">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K14">
+      <c r="L14">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C15">
         <v>200000</v>
@@ -972,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1">
         <v>43952</v>
@@ -980,25 +1080,31 @@
       <c r="G15" s="1">
         <v>44317</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="4">
+        <v>4</v>
+      </c>
+      <c r="J15">
         <v>0.4</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>1.8</v>
       </c>
-      <c r="J15">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K15">
+      <c r="L15">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <v>200000</v>
@@ -1007,7 +1113,7 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F16" s="1">
         <v>43952</v>
@@ -1015,25 +1121,31 @@
       <c r="G16" s="1">
         <v>44317</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="4">
+        <v>4</v>
+      </c>
+      <c r="J16">
         <v>0.5</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>1.9</v>
       </c>
-      <c r="J16">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K16">
+      <c r="L16">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M16">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>200000</v>
@@ -1042,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F17" s="1">
         <v>43952</v>
@@ -1050,25 +1162,31 @@
       <c r="G17" s="1">
         <v>44317</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="4">
+        <v>4</v>
+      </c>
+      <c r="J17">
         <v>0.6</v>
       </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-      <c r="J17">
-        <v>7.5000000000000002E-4</v>
-      </c>
       <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M17">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18">
         <v>200000</v>
@@ -1077,7 +1195,7 @@
         <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1">
         <v>43952</v>
@@ -1085,25 +1203,31 @@
       <c r="G18" s="1">
         <v>44317</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="4">
+        <v>4</v>
+      </c>
+      <c r="J18">
         <v>0.7</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>2.1</v>
       </c>
-      <c r="J18">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K18">
+      <c r="L18">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M18">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <v>200000</v>
@@ -1112,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F19" s="1">
         <v>43952</v>
@@ -1120,25 +1244,31 @@
       <c r="G19" s="1">
         <v>44317</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="4">
+        <v>4</v>
+      </c>
+      <c r="J19">
         <v>0.8</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J19">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K19">
+      <c r="L19">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M19">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C20">
         <v>200000</v>
@@ -1147,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F20" s="1">
         <v>43952</v>
@@ -1155,25 +1285,31 @@
       <c r="G20" s="1">
         <v>44317</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="4">
+        <v>4</v>
+      </c>
+      <c r="J20">
         <v>0.9</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J20">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K20">
+      <c r="L20">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <v>200000</v>
@@ -1182,7 +1318,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F21" s="1">
         <v>43952</v>
@@ -1190,25 +1326,31 @@
       <c r="G21" s="1">
         <v>44317</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="4">
+        <v>4</v>
+      </c>
+      <c r="J21">
         <v>1</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>2.4</v>
       </c>
-      <c r="J21">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K21">
+      <c r="L21">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M21">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>200000</v>
@@ -1217,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F22" s="1">
         <v>43952</v>
@@ -1225,25 +1367,31 @@
       <c r="G22" s="1">
         <v>44317</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I22" s="4">
+        <v>4</v>
+      </c>
+      <c r="J22">
         <v>0.1</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>1.5</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>1E-3</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C23">
         <v>200000</v>
@@ -1252,7 +1400,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F23" s="1">
         <v>43952</v>
@@ -1260,25 +1408,31 @@
       <c r="G23" s="1">
         <v>44317</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="4">
+        <v>4</v>
+      </c>
+      <c r="J23">
         <v>0.2</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>1.6</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>1E-3</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>200000</v>
@@ -1287,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F24" s="1">
         <v>43952</v>
@@ -1295,25 +1449,31 @@
       <c r="G24" s="1">
         <v>44317</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="4">
+        <v>4</v>
+      </c>
+      <c r="J24">
         <v>0.3</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>1.7</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>1E-3</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C25">
         <v>200000</v>
@@ -1322,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F25" s="1">
         <v>43952</v>
@@ -1330,25 +1490,31 @@
       <c r="G25" s="1">
         <v>44317</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" s="4">
+        <v>4</v>
+      </c>
+      <c r="J25">
         <v>0.4</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>1.8</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>1E-3</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C26">
         <v>200000</v>
@@ -1357,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F26" s="1">
         <v>43952</v>
@@ -1365,25 +1531,31 @@
       <c r="G26" s="1">
         <v>44317</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="4">
+        <v>4</v>
+      </c>
+      <c r="J26">
         <v>0.5</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>1.9</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>1E-3</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>200000</v>
@@ -1392,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F27" s="1">
         <v>43952</v>
@@ -1400,25 +1572,31 @@
       <c r="G27" s="1">
         <v>44317</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27" s="4">
+        <v>4</v>
+      </c>
+      <c r="J27">
         <v>0.6</v>
       </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-      <c r="J27">
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
         <v>1E-3</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>200000</v>
@@ -1427,7 +1605,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F28" s="1">
         <v>43952</v>
@@ -1435,25 +1613,31 @@
       <c r="G28" s="1">
         <v>44317</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="4">
+        <v>4</v>
+      </c>
+      <c r="J28">
         <v>0.7</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>2.1</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>1E-3</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C29">
         <v>200000</v>
@@ -1462,7 +1646,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F29" s="1">
         <v>43952</v>
@@ -1470,25 +1654,31 @@
       <c r="G29" s="1">
         <v>44317</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29" s="4">
+        <v>4</v>
+      </c>
+      <c r="J29">
         <v>0.8</v>
       </c>
-      <c r="I29">
+      <c r="K29">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>1E-3</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <v>200000</v>
@@ -1497,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F30" s="1">
         <v>43952</v>
@@ -1505,25 +1695,31 @@
       <c r="G30" s="1">
         <v>44317</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="4">
+        <v>4</v>
+      </c>
+      <c r="J30">
         <v>0.9</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>1E-3</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>200000</v>
@@ -1532,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F31" s="1">
         <v>43952</v>
@@ -1540,25 +1736,31 @@
       <c r="G31" s="1">
         <v>44317</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="4">
+        <v>4</v>
+      </c>
+      <c r="J31">
         <v>1</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <v>2.4</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>1E-3</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C32">
         <v>200000</v>
@@ -1567,7 +1769,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F32" s="1">
         <v>43952</v>
@@ -1575,25 +1777,31 @@
       <c r="G32" s="1">
         <v>44317</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="4">
+        <v>4</v>
+      </c>
+      <c r="J32">
         <v>0.1</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>1.5</v>
       </c>
-      <c r="J32">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C33">
         <v>200000</v>
@@ -1602,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1">
         <v>43952</v>
@@ -1610,25 +1818,31 @@
       <c r="G33" s="1">
         <v>44317</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="4">
+        <v>4</v>
+      </c>
+      <c r="J33">
         <v>0.2</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>1.6</v>
       </c>
-      <c r="J33">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>200000</v>
@@ -1637,7 +1851,7 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F34" s="1">
         <v>43952</v>
@@ -1645,25 +1859,31 @@
       <c r="G34" s="1">
         <v>44317</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" s="4">
+        <v>4</v>
+      </c>
+      <c r="J34">
         <v>0.3</v>
       </c>
-      <c r="I34">
+      <c r="K34">
         <v>1.7</v>
       </c>
-      <c r="J34">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K34">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C35">
         <v>200000</v>
@@ -1672,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F35" s="1">
         <v>43952</v>
@@ -1680,25 +1900,31 @@
       <c r="G35" s="1">
         <v>44317</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="4">
+        <v>4</v>
+      </c>
+      <c r="J35">
         <v>0.4</v>
       </c>
-      <c r="I35">
+      <c r="K35">
         <v>1.8</v>
       </c>
-      <c r="J35">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C36">
         <v>200000</v>
@@ -1707,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F36" s="1">
         <v>43952</v>
@@ -1715,25 +1941,31 @@
       <c r="G36" s="1">
         <v>44317</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="4">
+        <v>4</v>
+      </c>
+      <c r="J36">
         <v>0.5</v>
       </c>
-      <c r="I36">
+      <c r="K36">
         <v>1.9</v>
       </c>
-      <c r="J36">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <v>200000</v>
@@ -1742,7 +1974,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F37" s="1">
         <v>43952</v>
@@ -1750,25 +1982,31 @@
       <c r="G37" s="1">
         <v>44317</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="4">
+        <v>4</v>
+      </c>
+      <c r="J37">
         <v>0.6</v>
       </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-      <c r="J37">
-        <v>7.5000000000000002E-4</v>
-      </c>
       <c r="K37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C38">
         <v>200000</v>
@@ -1777,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>43952</v>
@@ -1785,25 +2023,31 @@
       <c r="G38" s="1">
         <v>44317</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="4">
+        <v>4</v>
+      </c>
+      <c r="J38">
         <v>0.7</v>
       </c>
-      <c r="I38">
+      <c r="K38">
         <v>2.1</v>
       </c>
-      <c r="J38">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K38">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C39">
         <v>200000</v>
@@ -1812,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F39" s="1">
         <v>43952</v>
@@ -1820,25 +2064,31 @@
       <c r="G39" s="1">
         <v>44317</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39" s="4">
+        <v>4</v>
+      </c>
+      <c r="J39">
         <v>0.8</v>
       </c>
-      <c r="I39">
+      <c r="K39">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J39">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C40">
         <v>200000</v>
@@ -1847,7 +2097,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F40" s="1">
         <v>43952</v>
@@ -1855,25 +2105,31 @@
       <c r="G40" s="1">
         <v>44317</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="4">
+        <v>4</v>
+      </c>
+      <c r="J40">
         <v>0.9</v>
       </c>
-      <c r="I40">
+      <c r="K40">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J40">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C41">
         <v>200000</v>
@@ -1882,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F41" s="1">
         <v>43952</v>
@@ -1890,25 +2146,31 @@
       <c r="G41" s="1">
         <v>44317</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="4">
+        <v>4</v>
+      </c>
+      <c r="J41">
         <v>1</v>
       </c>
-      <c r="I41">
+      <c r="K41">
         <v>2.4</v>
       </c>
-      <c r="J41">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C42">
         <v>200000</v>
@@ -1917,7 +2179,7 @@
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1">
         <v>43952</v>
@@ -1925,25 +2187,31 @@
       <c r="G42" s="1">
         <v>44317</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="4">
+        <v>4</v>
+      </c>
+      <c r="J42">
         <v>0.1</v>
       </c>
-      <c r="I42">
+      <c r="K42">
         <v>1.5</v>
       </c>
-      <c r="J42">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K42">
+      <c r="L42">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C43">
         <v>200000</v>
@@ -1952,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F43" s="1">
         <v>43952</v>
@@ -1960,25 +2228,31 @@
       <c r="G43" s="1">
         <v>44317</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43" s="4">
+        <v>4</v>
+      </c>
+      <c r="J43">
         <v>0.2</v>
       </c>
-      <c r="I43">
+      <c r="K43">
         <v>1.6</v>
       </c>
-      <c r="J43">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K43">
+      <c r="L43">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M43">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C44">
         <v>200000</v>
@@ -1987,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1">
         <v>43952</v>
@@ -1995,25 +2269,31 @@
       <c r="G44" s="1">
         <v>44317</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44" s="4">
+        <v>4</v>
+      </c>
+      <c r="J44">
         <v>0.3</v>
       </c>
-      <c r="I44">
+      <c r="K44">
         <v>1.7</v>
       </c>
-      <c r="J44">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K44">
+      <c r="L44">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C45">
         <v>200000</v>
@@ -2022,7 +2302,7 @@
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F45" s="1">
         <v>43952</v>
@@ -2030,25 +2310,31 @@
       <c r="G45" s="1">
         <v>44317</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="4">
+        <v>4</v>
+      </c>
+      <c r="J45">
         <v>0.4</v>
       </c>
-      <c r="I45">
+      <c r="K45">
         <v>1.8</v>
       </c>
-      <c r="J45">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K45">
+      <c r="L45">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M45">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>200000</v>
@@ -2057,7 +2343,7 @@
         <v>0</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1">
         <v>43952</v>
@@ -2065,25 +2351,31 @@
       <c r="G46" s="1">
         <v>44317</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="4">
+        <v>4</v>
+      </c>
+      <c r="J46">
         <v>0.5</v>
       </c>
-      <c r="I46">
+      <c r="K46">
         <v>1.9</v>
       </c>
-      <c r="J46">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K46">
+      <c r="L46">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M46">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C47">
         <v>200000</v>
@@ -2092,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F47" s="1">
         <v>43952</v>
@@ -2100,25 +2392,31 @@
       <c r="G47" s="1">
         <v>44317</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="4">
+        <v>4</v>
+      </c>
+      <c r="J47">
         <v>0.6</v>
       </c>
-      <c r="I47">
-        <v>2</v>
-      </c>
-      <c r="J47">
-        <v>7.5000000000000002E-4</v>
-      </c>
       <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M47">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C48">
         <v>200000</v>
@@ -2127,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F48" s="1">
         <v>43952</v>
@@ -2135,25 +2433,31 @@
       <c r="G48" s="1">
         <v>44317</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I48" s="4">
+        <v>4</v>
+      </c>
+      <c r="J48">
         <v>0.7</v>
       </c>
-      <c r="I48">
+      <c r="K48">
         <v>2.1</v>
       </c>
-      <c r="J48">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K48">
+      <c r="L48">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M48">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>200000</v>
@@ -2162,7 +2466,7 @@
         <v>0</v>
       </c>
       <c r="E49" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F49" s="1">
         <v>43952</v>
@@ -2170,25 +2474,31 @@
       <c r="G49" s="1">
         <v>44317</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" s="4">
+        <v>4</v>
+      </c>
+      <c r="J49">
         <v>0.8</v>
       </c>
-      <c r="I49">
+      <c r="K49">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J49">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K49">
+      <c r="L49">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M49">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C50">
         <v>200000</v>
@@ -2197,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F50" s="1">
         <v>43952</v>
@@ -2205,25 +2515,31 @@
       <c r="G50" s="1">
         <v>44317</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="4">
+        <v>4</v>
+      </c>
+      <c r="J50">
         <v>0.9</v>
       </c>
-      <c r="I50">
+      <c r="K50">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J50">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K50">
+      <c r="L50">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M50">
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C51">
         <v>200000</v>
@@ -2232,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F51" s="1">
         <v>43952</v>
@@ -2240,25 +2556,31 @@
       <c r="G51" s="1">
         <v>44317</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="4">
+        <v>4</v>
+      </c>
+      <c r="J51">
         <v>1</v>
       </c>
-      <c r="I51">
+      <c r="K51">
         <v>2.4</v>
       </c>
-      <c r="J51">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K51">
+      <c r="L51">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M51">
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C52">
         <v>200000</v>
@@ -2267,7 +2589,7 @@
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F52" s="1">
         <v>43952</v>
@@ -2275,25 +2597,31 @@
       <c r="G52" s="1">
         <v>44317</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="4">
+        <v>4</v>
+      </c>
+      <c r="J52">
         <v>0.1</v>
       </c>
-      <c r="I52">
+      <c r="K52">
         <v>1.5</v>
       </c>
-      <c r="J52">
+      <c r="L52">
         <v>1E-3</v>
       </c>
-      <c r="K52">
+      <c r="M52">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C53">
         <v>200000</v>
@@ -2302,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F53" s="1">
         <v>43952</v>
@@ -2310,25 +2638,31 @@
       <c r="G53" s="1">
         <v>44317</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="4">
+        <v>4</v>
+      </c>
+      <c r="J53">
         <v>0.2</v>
       </c>
-      <c r="I53">
+      <c r="K53">
         <v>1.6</v>
       </c>
-      <c r="J53">
+      <c r="L53">
         <v>1E-3</v>
       </c>
-      <c r="K53">
+      <c r="M53">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C54">
         <v>200000</v>
@@ -2337,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F54" s="1">
         <v>43952</v>
@@ -2345,25 +2679,31 @@
       <c r="G54" s="1">
         <v>44317</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="4">
+        <v>4</v>
+      </c>
+      <c r="J54">
         <v>0.3</v>
       </c>
-      <c r="I54">
+      <c r="K54">
         <v>1.7</v>
       </c>
-      <c r="J54">
+      <c r="L54">
         <v>1E-3</v>
       </c>
-      <c r="K54">
+      <c r="M54">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C55">
         <v>200000</v>
@@ -2372,7 +2712,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F55" s="1">
         <v>43952</v>
@@ -2380,25 +2720,31 @@
       <c r="G55" s="1">
         <v>44317</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="4">
+        <v>4</v>
+      </c>
+      <c r="J55">
         <v>0.4</v>
       </c>
-      <c r="I55">
+      <c r="K55">
         <v>1.8</v>
       </c>
-      <c r="J55">
+      <c r="L55">
         <v>1E-3</v>
       </c>
-      <c r="K55">
+      <c r="M55">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C56">
         <v>200000</v>
@@ -2407,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F56" s="1">
         <v>43952</v>
@@ -2415,25 +2761,31 @@
       <c r="G56" s="1">
         <v>44317</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" s="4">
+        <v>4</v>
+      </c>
+      <c r="J56">
         <v>0.5</v>
       </c>
-      <c r="I56">
+      <c r="K56">
         <v>1.9</v>
       </c>
-      <c r="J56">
+      <c r="L56">
         <v>1E-3</v>
       </c>
-      <c r="K56">
+      <c r="M56">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C57">
         <v>200000</v>
@@ -2442,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F57" s="1">
         <v>43952</v>
@@ -2450,25 +2802,31 @@
       <c r="G57" s="1">
         <v>44317</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" s="4">
+        <v>4</v>
+      </c>
+      <c r="J57">
         <v>0.6</v>
       </c>
-      <c r="I57">
-        <v>2</v>
-      </c>
-      <c r="J57">
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="L57">
         <v>1E-3</v>
       </c>
-      <c r="K57">
+      <c r="M57">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C58">
         <v>200000</v>
@@ -2477,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F58" s="1">
         <v>43952</v>
@@ -2485,25 +2843,31 @@
       <c r="G58" s="1">
         <v>44317</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="4">
+        <v>4</v>
+      </c>
+      <c r="J58">
         <v>0.7</v>
       </c>
-      <c r="I58">
+      <c r="K58">
         <v>2.1</v>
       </c>
-      <c r="J58">
+      <c r="L58">
         <v>1E-3</v>
       </c>
-      <c r="K58">
+      <c r="M58">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>200000</v>
@@ -2512,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="E59" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F59" s="1">
         <v>43952</v>
@@ -2520,25 +2884,31 @@
       <c r="G59" s="1">
         <v>44317</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" s="4">
+        <v>4</v>
+      </c>
+      <c r="J59">
         <v>0.8</v>
       </c>
-      <c r="I59">
+      <c r="K59">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J59">
+      <c r="L59">
         <v>1E-3</v>
       </c>
-      <c r="K59">
+      <c r="M59">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C60">
         <v>200000</v>
@@ -2547,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F60" s="1">
         <v>43952</v>
@@ -2555,25 +2925,31 @@
       <c r="G60" s="1">
         <v>44317</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I60" s="4">
+        <v>4</v>
+      </c>
+      <c r="J60">
         <v>0.9</v>
       </c>
-      <c r="I60">
+      <c r="K60">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J60">
+      <c r="L60">
         <v>1E-3</v>
       </c>
-      <c r="K60">
+      <c r="M60">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C61">
         <v>200000</v>
@@ -2582,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F61" s="1">
         <v>43952</v>
@@ -2590,25 +2966,31 @@
       <c r="G61" s="1">
         <v>44317</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I61" s="4">
+        <v>4</v>
+      </c>
+      <c r="J61">
         <v>1</v>
       </c>
-      <c r="I61">
+      <c r="K61">
         <v>2.4</v>
       </c>
-      <c r="J61">
+      <c r="L61">
         <v>1E-3</v>
       </c>
-      <c r="K61">
+      <c r="M61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C62">
         <v>200000</v>
@@ -2617,7 +2999,7 @@
         <v>0</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F62" s="1">
         <v>43079</v>
@@ -2625,25 +3007,31 @@
       <c r="G62" s="1">
         <v>43191</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I62" s="4">
+        <v>4</v>
+      </c>
+      <c r="J62">
         <v>0.1</v>
       </c>
-      <c r="I62">
+      <c r="K62">
         <v>1.5</v>
       </c>
-      <c r="J62">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K62">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C63">
         <v>200000</v>
@@ -2652,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F63" s="1">
         <v>43079</v>
@@ -2660,25 +3048,31 @@
       <c r="G63" s="1">
         <v>43191</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I63" s="4">
+        <v>4</v>
+      </c>
+      <c r="J63">
         <v>0.2</v>
       </c>
-      <c r="I63">
+      <c r="K63">
         <v>1.6</v>
       </c>
-      <c r="J63">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K63">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C64">
         <v>200000</v>
@@ -2687,7 +3081,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F64" s="1">
         <v>43079</v>
@@ -2695,25 +3089,31 @@
       <c r="G64" s="1">
         <v>43191</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I64" s="4">
+        <v>4</v>
+      </c>
+      <c r="J64">
         <v>0.3</v>
       </c>
-      <c r="I64">
+      <c r="K64">
         <v>1.7</v>
       </c>
-      <c r="J64">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K64">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C65">
         <v>200000</v>
@@ -2722,7 +3122,7 @@
         <v>0</v>
       </c>
       <c r="E65" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F65" s="1">
         <v>43079</v>
@@ -2730,25 +3130,31 @@
       <c r="G65" s="1">
         <v>43191</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I65" s="4">
+        <v>4</v>
+      </c>
+      <c r="J65">
         <v>0.4</v>
       </c>
-      <c r="I65">
+      <c r="K65">
         <v>1.8</v>
       </c>
-      <c r="J65">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K65">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C66">
         <v>200000</v>
@@ -2757,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F66" s="1">
         <v>43079</v>
@@ -2765,25 +3171,31 @@
       <c r="G66" s="1">
         <v>43191</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I66" s="4">
+        <v>4</v>
+      </c>
+      <c r="J66">
         <v>0.5</v>
       </c>
-      <c r="I66">
+      <c r="K66">
         <v>1.9</v>
       </c>
-      <c r="J66">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C67">
         <v>200000</v>
@@ -2792,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="E67" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F67" s="1">
         <v>43079</v>
@@ -2800,25 +3212,31 @@
       <c r="G67" s="1">
         <v>43191</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I67" s="4">
+        <v>4</v>
+      </c>
+      <c r="J67">
         <v>0.6</v>
       </c>
-      <c r="I67">
-        <v>2</v>
-      </c>
-      <c r="J67">
-        <v>7.5000000000000002E-4</v>
-      </c>
       <c r="K67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L67">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C68">
         <v>200000</v>
@@ -2827,7 +3245,7 @@
         <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F68" s="1">
         <v>43079</v>
@@ -2835,25 +3253,31 @@
       <c r="G68" s="1">
         <v>43191</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I68" s="4">
+        <v>4</v>
+      </c>
+      <c r="J68">
         <v>0.7</v>
       </c>
-      <c r="I68">
+      <c r="K68">
         <v>2.1</v>
       </c>
-      <c r="J68">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C69">
         <v>200000</v>
@@ -2862,7 +3286,7 @@
         <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F69" s="1">
         <v>43079</v>
@@ -2870,25 +3294,31 @@
       <c r="G69" s="1">
         <v>43191</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I69" s="4">
+        <v>4</v>
+      </c>
+      <c r="J69">
         <v>0.8</v>
       </c>
-      <c r="I69">
+      <c r="K69">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J69">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L69">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C70">
         <v>200000</v>
@@ -2897,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F70" s="1">
         <v>43079</v>
@@ -2905,25 +3335,31 @@
       <c r="G70" s="1">
         <v>43191</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I70" s="4">
+        <v>4</v>
+      </c>
+      <c r="J70">
         <v>0.9</v>
       </c>
-      <c r="I70">
+      <c r="K70">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J70">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K70">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C71">
         <v>200000</v>
@@ -2932,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F71" s="1">
         <v>43079</v>
@@ -2940,25 +3376,31 @@
       <c r="G71" s="1">
         <v>43191</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I71" s="4">
+        <v>4</v>
+      </c>
+      <c r="J71">
         <v>1</v>
       </c>
-      <c r="I71">
+      <c r="K71">
         <v>2.4</v>
       </c>
-      <c r="J71">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L71">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C72">
         <v>200000</v>
@@ -2967,7 +3409,7 @@
         <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F72" s="1">
         <v>43106</v>
@@ -2975,25 +3417,31 @@
       <c r="G72" s="1">
         <v>43191</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I72" s="4">
+        <v>4</v>
+      </c>
+      <c r="J72">
         <v>0.1</v>
       </c>
-      <c r="I72">
+      <c r="K72">
         <v>1.5</v>
       </c>
-      <c r="J72">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C73">
         <v>200000</v>
@@ -3002,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F73" s="1">
         <v>43106</v>
@@ -3010,25 +3458,31 @@
       <c r="G73" s="1">
         <v>43191</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I73" s="4">
+        <v>4</v>
+      </c>
+      <c r="J73">
         <v>0.2</v>
       </c>
-      <c r="I73">
+      <c r="K73">
         <v>1.6</v>
       </c>
-      <c r="J73">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C74">
         <v>200000</v>
@@ -3037,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="E74" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F74" s="1">
         <v>43106</v>
@@ -3045,25 +3499,31 @@
       <c r="G74" s="1">
         <v>43191</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I74" s="4">
+        <v>4</v>
+      </c>
+      <c r="J74">
         <v>0.3</v>
       </c>
-      <c r="I74">
+      <c r="K74">
         <v>1.7</v>
       </c>
-      <c r="J74">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K74">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L74">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C75">
         <v>200000</v>
@@ -3072,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F75" s="1">
         <v>43106</v>
@@ -3080,25 +3540,31 @@
       <c r="G75" s="1">
         <v>43191</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I75" s="4">
+        <v>4</v>
+      </c>
+      <c r="J75">
         <v>0.4</v>
       </c>
-      <c r="I75">
+      <c r="K75">
         <v>1.8</v>
       </c>
-      <c r="J75">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K75">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C76">
         <v>200000</v>
@@ -3107,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="E76" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F76" s="1">
         <v>43106</v>
@@ -3115,25 +3581,31 @@
       <c r="G76" s="1">
         <v>43191</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I76" s="4">
+        <v>4</v>
+      </c>
+      <c r="J76">
         <v>0.5</v>
       </c>
-      <c r="I76">
+      <c r="K76">
         <v>1.9</v>
       </c>
-      <c r="J76">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C77">
         <v>200000</v>
@@ -3142,7 +3614,7 @@
         <v>0</v>
       </c>
       <c r="E77" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F77" s="1">
         <v>43106</v>
@@ -3150,25 +3622,31 @@
       <c r="G77" s="1">
         <v>43191</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I77" s="4">
+        <v>4</v>
+      </c>
+      <c r="J77">
         <v>0.6</v>
       </c>
-      <c r="I77">
-        <v>2</v>
-      </c>
-      <c r="J77">
-        <v>7.5000000000000002E-4</v>
-      </c>
       <c r="K77">
         <v>2</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C78">
         <v>200000</v>
@@ -3177,7 +3655,7 @@
         <v>0</v>
       </c>
       <c r="E78" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F78" s="1">
         <v>43106</v>
@@ -3185,25 +3663,31 @@
       <c r="G78" s="1">
         <v>43191</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I78" s="4">
+        <v>4</v>
+      </c>
+      <c r="J78">
         <v>0.7</v>
       </c>
-      <c r="I78">
+      <c r="K78">
         <v>2.1</v>
       </c>
-      <c r="J78">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K78">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C79">
         <v>200000</v>
@@ -3212,7 +3696,7 @@
         <v>0</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F79" s="1">
         <v>43106</v>
@@ -3220,25 +3704,31 @@
       <c r="G79" s="1">
         <v>43191</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I79" s="4">
+        <v>4</v>
+      </c>
+      <c r="J79">
         <v>0.8</v>
       </c>
-      <c r="I79">
+      <c r="K79">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J79">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C80">
         <v>200000</v>
@@ -3247,7 +3737,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F80" s="1">
         <v>43106</v>
@@ -3255,25 +3745,31 @@
       <c r="G80" s="1">
         <v>43191</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I80" s="4">
+        <v>4</v>
+      </c>
+      <c r="J80">
         <v>0.9</v>
       </c>
-      <c r="I80">
+      <c r="K80">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J80">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K80">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C81">
         <v>200000</v>
@@ -3282,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="E81" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F81" s="1">
         <v>43106</v>
@@ -3290,25 +3786,31 @@
       <c r="G81" s="1">
         <v>43191</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I81" s="4">
+        <v>4</v>
+      </c>
+      <c r="J81">
         <v>1</v>
       </c>
-      <c r="I81">
+      <c r="K81">
         <v>2.4</v>
       </c>
-      <c r="J81">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K81">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C82">
         <v>200000</v>
@@ -3317,7 +3819,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
         <v>44197</v>
@@ -3325,25 +3827,31 @@
       <c r="G82" s="1">
         <v>44308</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I82" s="4">
+        <v>4</v>
+      </c>
+      <c r="J82">
         <v>-6.12781991416309E-2</v>
       </c>
-      <c r="I82">
+      <c r="K82">
         <v>3.2731140296139101</v>
       </c>
-      <c r="J82">
+      <c r="L82">
         <v>4.4100133020519598E-3</v>
       </c>
-      <c r="K82">
+      <c r="M82">
         <v>0.94042482754768197</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C83">
         <v>200000</v>
@@ -3352,7 +3860,7 @@
         <v>0</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F83" s="1">
         <v>44197</v>
@@ -3360,25 +3868,31 @@
       <c r="G83" s="1">
         <v>44308</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I83" s="4">
+        <v>4</v>
+      </c>
+      <c r="J83">
         <v>9.7999647483704693E-3</v>
       </c>
-      <c r="I83">
+      <c r="K83">
         <v>0.46292753916427498</v>
       </c>
-      <c r="J83">
+      <c r="L83">
         <v>3.4255696986459101E-3</v>
       </c>
-      <c r="K83">
+      <c r="M83">
         <v>3.41461894440372</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C84">
         <v>200000</v>
@@ -3387,7 +3901,7 @@
         <v>0</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
         <v>44197</v>
@@ -3395,26 +3909,29 @@
       <c r="G84" s="1">
         <v>44308</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I84" s="4">
+        <v>4</v>
+      </c>
+      <c r="J84">
         <v>0.1</v>
       </c>
-      <c r="I84">
+      <c r="K84">
         <v>0.5</v>
       </c>
-      <c r="J84">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
-      <c r="B85" t="s">
-        <v>13</v>
-      </c>
       <c r="C85">
         <v>200000</v>
       </c>
@@ -3422,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1">
         <v>44309</v>
@@ -3430,29 +3947,32 @@
       <c r="G85" s="1">
         <v>44337</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I85" s="4">
+        <v>4</v>
+      </c>
+      <c r="J85">
         <v>7.1899967358760703E-4</v>
       </c>
-      <c r="I85">
+      <c r="K85">
         <v>0.331736520860619</v>
       </c>
-      <c r="J85">
+      <c r="L85">
         <v>2.3784997256206101E-3</v>
       </c>
-      <c r="K85">
+      <c r="M85">
         <v>3.0648528356896501</v>
       </c>
-      <c r="L85" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
-        <v>13</v>
-      </c>
       <c r="C86">
         <v>200000</v>
       </c>
@@ -3460,7 +3980,7 @@
         <v>0</v>
       </c>
       <c r="E86" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F86" s="1">
         <v>44309</v>
@@ -3468,23 +3988,29 @@
       <c r="G86" s="1">
         <v>44337</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I86" s="4">
+        <v>4</v>
+      </c>
+      <c r="J86">
         <v>0.01</v>
       </c>
-      <c r="I86">
+      <c r="K86">
         <v>0.5</v>
       </c>
-      <c r="J86">
-        <v>7.5000000000000002E-4</v>
-      </c>
-      <c r="K86">
-        <v>2</v>
-      </c>
-      <c r="L86" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="M86">
+        <v>2</v>
+      </c>
+      <c r="N86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3495,7 +4021,7 @@
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F87" s="1">
         <v>44309</v>
@@ -3503,28 +4029,34 @@
       <c r="G87" s="1">
         <v>44337</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I87" s="4">
+        <v>4</v>
+      </c>
+      <c r="J87">
         <v>7.7137627095034397E-2</v>
       </c>
-      <c r="I87">
+      <c r="K87">
         <v>0.147341631456371</v>
       </c>
-      <c r="J87">
+      <c r="L87">
         <v>3.3881238556444401E-3</v>
       </c>
-      <c r="K87">
+      <c r="M87">
         <v>0.58523196662204202</v>
       </c>
-      <c r="L87" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C88">
         <v>200000</v>
@@ -3533,7 +4065,7 @@
         <v>0</v>
       </c>
       <c r="E88" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F88" s="1">
         <v>43106</v>
@@ -3541,25 +4073,31 @@
       <c r="G88" s="1">
         <v>43191</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I88" s="4">
+        <v>4</v>
+      </c>
+      <c r="J88">
         <v>7.7137627095034397E-2</v>
       </c>
-      <c r="I88">
+      <c r="K88">
         <v>0.147341631456371</v>
       </c>
-      <c r="J88">
+      <c r="L88">
         <v>3.3881238556444401E-3</v>
       </c>
-      <c r="K88">
+      <c r="M88">
         <v>0.58523196662204202</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C89">
         <v>200000</v>
@@ -3568,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1">
         <v>44311</v>
@@ -3576,28 +4114,34 @@
       <c r="G89" s="1">
         <v>44336</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I89" s="4">
+        <v>4</v>
+      </c>
+      <c r="J89">
         <v>4.8883000000000003E-2</v>
       </c>
-      <c r="I89">
+      <c r="K89">
         <v>0.18237500000000001</v>
       </c>
-      <c r="J89">
+      <c r="L89">
         <v>3.6870000000000002E-3</v>
       </c>
-      <c r="K89">
+      <c r="M89">
         <v>6.1486150000000004</v>
       </c>
-      <c r="L89" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N89" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C90">
         <v>200000</v>
@@ -3606,7 +4150,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F90" s="1">
         <v>44200</v>
@@ -3614,25 +4158,31 @@
       <c r="G90" s="1">
         <v>44247</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I90" s="4">
+        <v>4</v>
+      </c>
+      <c r="J90">
         <v>4.8883000000000003E-2</v>
       </c>
-      <c r="I90">
+      <c r="K90">
         <v>0.18237500000000001</v>
       </c>
-      <c r="J90">
+      <c r="L90">
         <v>3.6870000000000002E-3</v>
       </c>
-      <c r="K90">
+      <c r="M90">
         <v>6.1486150000000004</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C91">
         <v>200000</v>
@@ -3641,7 +4191,7 @@
         <v>0</v>
       </c>
       <c r="E91" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F91" s="1">
         <v>44311</v>
@@ -3649,28 +4199,34 @@
       <c r="G91" s="1">
         <v>44336</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I91" s="4">
+        <v>4</v>
+      </c>
+      <c r="J91">
         <v>0.122063</v>
       </c>
-      <c r="I91">
+      <c r="K91">
         <v>0.143455</v>
       </c>
-      <c r="J91">
+      <c r="L91">
         <v>3.6110000000000001E-3</v>
       </c>
-      <c r="K91">
+      <c r="M91">
         <v>2.8670789999999999</v>
       </c>
-      <c r="L91" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N91" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C92">
         <v>200000</v>
@@ -3679,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="E92" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1">
         <v>44200</v>
@@ -3687,25 +4243,31 @@
       <c r="G92" s="1">
         <v>44247</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I92" s="4">
+        <v>4</v>
+      </c>
+      <c r="J92">
         <v>0.122063</v>
       </c>
-      <c r="I92">
+      <c r="K92">
         <v>0.143455</v>
       </c>
-      <c r="J92">
+      <c r="L92">
         <v>3.6110000000000001E-3</v>
       </c>
-      <c r="K92">
+      <c r="M92">
         <v>2.8670789999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C93">
         <v>200000</v>
@@ -3714,7 +4276,7 @@
         <v>0</v>
       </c>
       <c r="E93" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F93" s="1">
         <v>44200</v>
@@ -3722,17 +4284,58 @@
       <c r="G93" s="1">
         <v>44247</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I93" s="4">
+        <v>4</v>
+      </c>
+      <c r="J93">
         <v>0.61594599999999999</v>
       </c>
-      <c r="I93">
+      <c r="K93">
         <v>0.99924900000000005</v>
       </c>
-      <c r="J93">
+      <c r="L93">
         <v>8.1560000000000001E-3</v>
       </c>
-      <c r="K93">
+      <c r="M93">
         <v>0.74069700000000005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <v>200000</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>6</v>
+      </c>
+      <c r="F94" s="1">
+        <v>44309</v>
+      </c>
+      <c r="G94" s="1">
+        <v>44337</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I94" s="4">
+        <v>3</v>
+      </c>
+      <c r="J94">
+        <v>6.7664951384996105E-2</v>
+      </c>
+      <c r="K94">
+        <v>0.14299286941025699</v>
+      </c>
+      <c r="L94">
+        <v>2.7738933629813798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>